<commit_message>
completed insert into db from excel
also detect duplicates
</commit_message>
<xml_diff>
--- a/staff/SAMPLE DATA 1 EXCEL (STUDENT) - Copy.xlsx
+++ b/staff/SAMPLE DATA 1 EXCEL (STUDENT) - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\csc578_grp\staff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{176C1338-D8BA-489C-AB16-A5C57530319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F39E7-8B9E-4107-98AE-99EE1872C989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4597868-CF51-4A2D-94A3-6B0933786C32}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>student_BC</t>
   </si>
@@ -46,37 +46,7 @@
     <t>QWE123</t>
   </si>
   <si>
-    <t>QWE456</t>
-  </si>
-  <si>
-    <t>QWE789</t>
-  </si>
-  <si>
-    <t>RTY123</t>
-  </si>
-  <si>
-    <t>RTY456</t>
-  </si>
-  <si>
-    <t>RTY789</t>
-  </si>
-  <si>
     <t>TAEYON</t>
-  </si>
-  <si>
-    <t>SUNNY</t>
-  </si>
-  <si>
-    <t>SEJEONG</t>
-  </si>
-  <si>
-    <t>MINYEONG</t>
-  </si>
-  <si>
-    <t>SOLAR</t>
-  </si>
-  <si>
-    <t>HWASA</t>
   </si>
 </sst>
 </file>
@@ -439,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A624D-9243-49EF-8AF3-5A5BA33BC88D}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B7" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,47 +434,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>